<commit_message>
RS: updated 2024 pre-arb bonus and jan 2025 service time info
</commit_message>
<xml_diff>
--- a/data/PreArbBonus.xlsx
+++ b/data/PreArbBonus.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LK296/Documents/Research/Baseball/PreArbBonuses/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LK296/Documents/Research/Baseball/Pre-Arb Bonuses/Bonuses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5904A4-F6DA-A344-8A55-82C197A872D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4A1D0D-4849-D249-A2C3-E2D2A798641A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="15760" xr2:uid="{2DCACD9D-06F4-5342-9637-598D18DD3FC4}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="15760" activeTab="2" xr2:uid="{2DCACD9D-06F4-5342-9637-598D18DD3FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="BonusesAdj22" sheetId="5" r:id="rId1"/>
     <sheet name="BonusesAdj23" sheetId="3" r:id="rId2"/>
+    <sheet name="BonusesAdj24" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="386">
   <si>
     <t>Julio Rodríguez</t>
   </si>
@@ -793,6 +794,408 @@
   </si>
   <si>
     <t>gonsoto01</t>
+  </si>
+  <si>
+    <t>Paul Skenes</t>
+  </si>
+  <si>
+    <t>Jackson Merrill</t>
+  </si>
+  <si>
+    <t>Luis Gil</t>
+  </si>
+  <si>
+    <t>Colton Cowser</t>
+  </si>
+  <si>
+    <t>Jackson Chourio</t>
+  </si>
+  <si>
+    <t>Mason Miller</t>
+  </si>
+  <si>
+    <t>Austin Wells</t>
+  </si>
+  <si>
+    <t>Cade Smith</t>
+  </si>
+  <si>
+    <t>Tanner Houck</t>
+  </si>
+  <si>
+    <t>Hunter Greene</t>
+  </si>
+  <si>
+    <t>Brenton Doyle</t>
+  </si>
+  <si>
+    <t>Oneil Cruz</t>
+  </si>
+  <si>
+    <t>Ronel Blanco</t>
+  </si>
+  <si>
+    <t>Masyn Winn</t>
+  </si>
+  <si>
+    <t>Zach Neto</t>
+  </si>
+  <si>
+    <t>Brendan Donovan</t>
+  </si>
+  <si>
+    <t>Lawrence Butler</t>
+  </si>
+  <si>
+    <t>Hunter Brown</t>
+  </si>
+  <si>
+    <t>Jake McCarthy</t>
+  </si>
+  <si>
+    <t>Tyler Fitzgerald</t>
+  </si>
+  <si>
+    <t>Ryan Walker</t>
+  </si>
+  <si>
+    <t>JJ Bleday</t>
+  </si>
+  <si>
+    <t>Mark Vientos</t>
+  </si>
+  <si>
+    <t>Wyatt Langford</t>
+  </si>
+  <si>
+    <t>Wilyer Abreu</t>
+  </si>
+  <si>
+    <t>Brice Turang</t>
+  </si>
+  <si>
+    <t>Spencer Schwellenbach</t>
+  </si>
+  <si>
+    <t>Bryan Woo</t>
+  </si>
+  <si>
+    <t>Griffin Jax</t>
+  </si>
+  <si>
+    <t>Gavin Stone</t>
+  </si>
+  <si>
+    <t>Pete Crow-Armstrong</t>
+  </si>
+  <si>
+    <t>Otto Lopez</t>
+  </si>
+  <si>
+    <t>Jacob Young</t>
+  </si>
+  <si>
+    <t>Josh Smith</t>
+  </si>
+  <si>
+    <t>Michael Busch</t>
+  </si>
+  <si>
+    <t>Jordan Westburg</t>
+  </si>
+  <si>
+    <t>Heliot Ramos</t>
+  </si>
+  <si>
+    <t>Xavier Edwards</t>
+  </si>
+  <si>
+    <t>Tobias Myers</t>
+  </si>
+  <si>
+    <t>MacKenzie Gore</t>
+  </si>
+  <si>
+    <t>Hunter Gaddis</t>
+  </si>
+  <si>
+    <t>Iván Herrera</t>
+  </si>
+  <si>
+    <t>Parker Meadows</t>
+  </si>
+  <si>
+    <t>Ryne Nelson</t>
+  </si>
+  <si>
+    <t>Brandon Pfaadt</t>
+  </si>
+  <si>
+    <t>Logan O’Hoppe</t>
+  </si>
+  <si>
+    <t>Reese Olson</t>
+  </si>
+  <si>
+    <t>Andre Pallante</t>
+  </si>
+  <si>
+    <t>Matt Wallner</t>
+  </si>
+  <si>
+    <t>Shea Langeliers</t>
+  </si>
+  <si>
+    <t>Garrett Mitchell</t>
+  </si>
+  <si>
+    <t>Bryan Hudson</t>
+  </si>
+  <si>
+    <t>Luis Ortiz</t>
+  </si>
+  <si>
+    <t>Ernie Clement</t>
+  </si>
+  <si>
+    <t>Colt Keith</t>
+  </si>
+  <si>
+    <t>Ryan Feltner</t>
+  </si>
+  <si>
+    <t>Spencer Horwitz</t>
+  </si>
+  <si>
+    <t>David Fry</t>
+  </si>
+  <si>
+    <t>Jake Irvin</t>
+  </si>
+  <si>
+    <t>Freddy Fermin</t>
+  </si>
+  <si>
+    <t>Sal Frelick</t>
+  </si>
+  <si>
+    <t>ROY</t>
+  </si>
+  <si>
+    <t>MVP-2; MLB-1</t>
+  </si>
+  <si>
+    <t>ROY; CY-3; MLB-1</t>
+  </si>
+  <si>
+    <t>skenepa01</t>
+  </si>
+  <si>
+    <t>MVP-5; MLB-1</t>
+  </si>
+  <si>
+    <t>MLB-2</t>
+  </si>
+  <si>
+    <t>merrija01</t>
+  </si>
+  <si>
+    <t>ROY-2; MLB-2</t>
+  </si>
+  <si>
+    <t>gillu01</t>
+  </si>
+  <si>
+    <t>cowseco01</t>
+  </si>
+  <si>
+    <t>chourja01</t>
+  </si>
+  <si>
+    <t>millema03</t>
+  </si>
+  <si>
+    <t>wellsau01</t>
+  </si>
+  <si>
+    <t>smithca06</t>
+  </si>
+  <si>
+    <t>houckta01</t>
+  </si>
+  <si>
+    <t>greenhu01</t>
+  </si>
+  <si>
+    <t>doylebr02</t>
+  </si>
+  <si>
+    <t>cruzon01</t>
+  </si>
+  <si>
+    <t>blancro01</t>
+  </si>
+  <si>
+    <t>winnma01</t>
+  </si>
+  <si>
+    <t>netoza01</t>
+  </si>
+  <si>
+    <t>ortizjo06</t>
+  </si>
+  <si>
+    <t>Joey Ortiz</t>
+  </si>
+  <si>
+    <t>donovbr01</t>
+  </si>
+  <si>
+    <t>butlela01</t>
+  </si>
+  <si>
+    <t>brownhu01</t>
+  </si>
+  <si>
+    <t>mccarja02</t>
+  </si>
+  <si>
+    <t>fitzgty01</t>
+  </si>
+  <si>
+    <t>walkery01</t>
+  </si>
+  <si>
+    <t>bledajj01</t>
+  </si>
+  <si>
+    <t>vientma01</t>
+  </si>
+  <si>
+    <t>langfwy01</t>
+  </si>
+  <si>
+    <t>abreuwi02</t>
+  </si>
+  <si>
+    <t>turanbr02</t>
+  </si>
+  <si>
+    <t>schwesp01</t>
+  </si>
+  <si>
+    <t>woobr01</t>
+  </si>
+  <si>
+    <t>jaxgr01</t>
+  </si>
+  <si>
+    <t>stonega01</t>
+  </si>
+  <si>
+    <t>crowape01</t>
+  </si>
+  <si>
+    <t>lopezot01</t>
+  </si>
+  <si>
+    <t>youngja03</t>
+  </si>
+  <si>
+    <t>smithjo11</t>
+  </si>
+  <si>
+    <t>buschmi02</t>
+  </si>
+  <si>
+    <t>westbjo01</t>
+  </si>
+  <si>
+    <t>ramoshe02</t>
+  </si>
+  <si>
+    <t>edwarxa01</t>
+  </si>
+  <si>
+    <t>myersto01</t>
+  </si>
+  <si>
+    <t>gorema01</t>
+  </si>
+  <si>
+    <t>gaddihu01</t>
+  </si>
+  <si>
+    <t>herreiv01</t>
+  </si>
+  <si>
+    <t>meadopa01</t>
+  </si>
+  <si>
+    <t>nelsory01</t>
+  </si>
+  <si>
+    <t>pfaadbr01</t>
+  </si>
+  <si>
+    <t>ohopplo01</t>
+  </si>
+  <si>
+    <t>olsonre01</t>
+  </si>
+  <si>
+    <t>pallaan01</t>
+  </si>
+  <si>
+    <t>wallnma01</t>
+  </si>
+  <si>
+    <t>langesh01</t>
+  </si>
+  <si>
+    <t>mitchga01</t>
+  </si>
+  <si>
+    <t>hudsobr01</t>
+  </si>
+  <si>
+    <t>ortizlu03</t>
+  </si>
+  <si>
+    <t>clemeer01</t>
+  </si>
+  <si>
+    <t>Simeon Woods Richardson</t>
+  </si>
+  <si>
+    <t>woodssi01</t>
+  </si>
+  <si>
+    <t>keithco01</t>
+  </si>
+  <si>
+    <t>feltnry01</t>
+  </si>
+  <si>
+    <t>horwisp01</t>
+  </si>
+  <si>
+    <t>fryda01</t>
+  </si>
+  <si>
+    <t>irvinja01</t>
+  </si>
+  <si>
+    <t>pepiory01</t>
+  </si>
+  <si>
+    <t>Ryan Pepiot</t>
+  </si>
+  <si>
+    <t>fermifr01</t>
+  </si>
+  <si>
+    <t>frelisa01</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22754D2-C9BA-0A4A-A346-B4CA85C93B22}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2033,7 +2436,7 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3814,4 +4217,1789 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C9B84E-834F-5B4C-8F9E-38BAFB9905EF}">
+  <dimension ref="A1:F102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>3077595</v>
+      </c>
+      <c r="C2">
+        <v>1750000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3">
+        <v>2152057</v>
+      </c>
+      <c r="C3">
+        <v>1500000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2007178</v>
+      </c>
+      <c r="C4">
+        <v>1000000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1722174</v>
+      </c>
+      <c r="C5">
+        <v>1000000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>317</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>1638013</v>
+      </c>
+      <c r="C6">
+        <v>100000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>1321661</v>
+      </c>
+      <c r="C7">
+        <v>500000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8">
+        <v>1191534</v>
+      </c>
+      <c r="C8">
+        <v>500000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" t="s">
+        <v>319</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9">
+        <v>1098628</v>
+      </c>
+      <c r="C9">
+        <v>750000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E9" t="s">
+        <v>321</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10">
+        <v>978671</v>
+      </c>
+      <c r="C10">
+        <v>500000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" t="s">
+        <v>322</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B11">
+        <v>901335</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12">
+        <v>860710</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B13">
+        <v>825276</v>
+      </c>
+      <c r="C13">
+        <v>500000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>318</v>
+      </c>
+      <c r="E13" t="s">
+        <v>324</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14">
+        <v>801564</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>325</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>713720</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16">
+        <v>687804</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>576282</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>194</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18">
+        <v>557688</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>326</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>555553</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>535533</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>260</v>
+      </c>
+      <c r="B21">
+        <v>534267</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>327</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>261</v>
+      </c>
+      <c r="B22">
+        <v>529910</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>328</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <v>517846</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>509957</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25">
+        <v>497306</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26">
+        <v>485706</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>201</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>262</v>
+      </c>
+      <c r="B27">
+        <v>484750</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>329</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>263</v>
+      </c>
+      <c r="B28">
+        <v>483928</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>330</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>264</v>
+      </c>
+      <c r="B29">
+        <v>473026</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>331</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>471042</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>156</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31">
+        <v>459896</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>332</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>446287</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>266</v>
+      </c>
+      <c r="B33">
+        <v>442551</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>333</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>335</v>
+      </c>
+      <c r="B34">
+        <v>427663</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>334</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35">
+        <v>424722</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>336</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36">
+        <v>418864</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>214</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>268</v>
+      </c>
+      <c r="B37">
+        <v>417995</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>337</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38">
+        <v>416842</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>338</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>270</v>
+      </c>
+      <c r="B39">
+        <v>414638</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>339</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>411884</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41">
+        <v>409573</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>340</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>272</v>
+      </c>
+      <c r="B42">
+        <v>382315</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>341</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43">
+        <v>381085</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>273</v>
+      </c>
+      <c r="B44">
+        <v>377494</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>342</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>274</v>
+      </c>
+      <c r="B45">
+        <v>370770</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>343</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>275</v>
+      </c>
+      <c r="B46">
+        <v>368844</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>344</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>276</v>
+      </c>
+      <c r="B47">
+        <v>368745</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>345</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>277</v>
+      </c>
+      <c r="B48">
+        <v>368014</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>346</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>278</v>
+      </c>
+      <c r="B49">
+        <v>365752</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>347</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>279</v>
+      </c>
+      <c r="B50">
+        <v>362483</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>348</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51">
+        <v>353159</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>154</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>280</v>
+      </c>
+      <c r="B52">
+        <v>352852</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>349</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>281</v>
+      </c>
+      <c r="B53">
+        <v>350022</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>350</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>282</v>
+      </c>
+      <c r="B54">
+        <v>342128</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>351</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55">
+        <v>341542</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>174</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>283</v>
+      </c>
+      <c r="B56">
+        <v>339964</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>352</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>284</v>
+      </c>
+      <c r="B57">
+        <v>333239</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>353</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>285</v>
+      </c>
+      <c r="B58">
+        <v>333175</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>354</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59">
+        <v>331054</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>168</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60">
+        <v>327719</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>211</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>286</v>
+      </c>
+      <c r="B61">
+        <v>325723</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>355</v>
+      </c>
+      <c r="F61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62">
+        <v>323520</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>162</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63">
+        <v>322695</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>203</v>
+      </c>
+      <c r="F63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>287</v>
+      </c>
+      <c r="B64">
+        <v>321013</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>356</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>288</v>
+      </c>
+      <c r="B65">
+        <v>314708</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>357</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66">
+        <v>314051</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>136</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>289</v>
+      </c>
+      <c r="B67">
+        <v>313489</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>358</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>45</v>
+      </c>
+      <c r="B68">
+        <v>312989</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>160</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>290</v>
+      </c>
+      <c r="B69">
+        <v>312411</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>359</v>
+      </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>58</v>
+      </c>
+      <c r="B70">
+        <v>310609</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>175</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>291</v>
+      </c>
+      <c r="B71">
+        <v>300017</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>360</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>292</v>
+      </c>
+      <c r="B72">
+        <v>291335</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>361</v>
+      </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>293</v>
+      </c>
+      <c r="B73">
+        <v>288414</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>362</v>
+      </c>
+      <c r="F73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>288310</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>116</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>48</v>
+      </c>
+      <c r="B75">
+        <v>277498</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>163</v>
+      </c>
+      <c r="F75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>294</v>
+      </c>
+      <c r="B76">
+        <v>276802</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>363</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>295</v>
+      </c>
+      <c r="B77">
+        <v>274561</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>364</v>
+      </c>
+      <c r="F77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>296</v>
+      </c>
+      <c r="B78">
+        <v>271783</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>365</v>
+      </c>
+      <c r="F78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79">
+        <v>267069</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>132</v>
+      </c>
+      <c r="F79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>297</v>
+      </c>
+      <c r="B80">
+        <v>263114</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>366</v>
+      </c>
+      <c r="F80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>298</v>
+      </c>
+      <c r="B81">
+        <v>261138</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>367</v>
+      </c>
+      <c r="F81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>299</v>
+      </c>
+      <c r="B82">
+        <v>260489</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>368</v>
+      </c>
+      <c r="F82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>300</v>
+      </c>
+      <c r="B83">
+        <v>256296</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>369</v>
+      </c>
+      <c r="F83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>301</v>
+      </c>
+      <c r="B84">
+        <v>255500</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>370</v>
+      </c>
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>302</v>
+      </c>
+      <c r="B85">
+        <v>254824</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>371</v>
+      </c>
+      <c r="F85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86">
+        <v>251338</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>127</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>303</v>
+      </c>
+      <c r="B87">
+        <v>246858</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>372</v>
+      </c>
+      <c r="F87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>304</v>
+      </c>
+      <c r="B88">
+        <v>246313</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>373</v>
+      </c>
+      <c r="F88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>305</v>
+      </c>
+      <c r="B89">
+        <v>245805</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>374</v>
+      </c>
+      <c r="F89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>96</v>
+      </c>
+      <c r="B90">
+        <v>245177</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>165</v>
+      </c>
+      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>375</v>
+      </c>
+      <c r="B91">
+        <v>243471</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="E91" t="s">
+        <v>376</v>
+      </c>
+      <c r="F91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>71</v>
+      </c>
+      <c r="B92">
+        <v>243098</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="E92" t="s">
+        <v>190</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>306</v>
+      </c>
+      <c r="B93">
+        <v>242569</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="E93" t="s">
+        <v>377</v>
+      </c>
+      <c r="F93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>307</v>
+      </c>
+      <c r="B94">
+        <v>241935</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>378</v>
+      </c>
+      <c r="F94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>308</v>
+      </c>
+      <c r="B95">
+        <v>241789</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>379</v>
+      </c>
+      <c r="F95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>68</v>
+      </c>
+      <c r="B96">
+        <v>241402</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="E96" t="s">
+        <v>187</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>309</v>
+      </c>
+      <c r="B97">
+        <v>240856</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>380</v>
+      </c>
+      <c r="F97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>310</v>
+      </c>
+      <c r="B98">
+        <v>239663</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>381</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>51</v>
+      </c>
+      <c r="B99">
+        <v>237986</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>167</v>
+      </c>
+      <c r="F99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>383</v>
+      </c>
+      <c r="B100">
+        <v>236029</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="E100" t="s">
+        <v>382</v>
+      </c>
+      <c r="F100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>311</v>
+      </c>
+      <c r="B101">
+        <v>232819</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="E101" t="s">
+        <v>384</v>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>312</v>
+      </c>
+      <c r="B102">
+        <v>232549</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="E102" t="s">
+        <v>385</v>
+      </c>
+      <c r="F102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stats import and initial comps
</commit_message>
<xml_diff>
--- a/data/PreArbBonus.xlsx
+++ b/data/PreArbBonus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LK296/Documents/Research/Baseball/Pre-Arb Bonuses/Bonuses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4A1D0D-4849-D249-A2C3-E2D2A798641A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128562E2-FAE3-D647-A237-796F38AD3C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="15760" activeTab="2" xr2:uid="{2DCACD9D-06F4-5342-9637-598D18DD3FC4}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="15760" xr2:uid="{2DCACD9D-06F4-5342-9637-598D18DD3FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="BonusesAdj22" sheetId="5" r:id="rId1"/>
@@ -379,9 +379,6 @@
     <t>ROY-1</t>
   </si>
   <si>
-    <t>BREFID</t>
-  </si>
-  <si>
     <t>rodriju01</t>
   </si>
   <si>
@@ -1196,6 +1193,9 @@
   </si>
   <si>
     <t>frelisa01</t>
+  </si>
+  <si>
+    <t>key_bbref</t>
   </si>
 </sst>
 </file>
@@ -1556,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22754D2-C9BA-0A4A-A346-B4CA85C93B22}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1579,15 +1579,15 @@
         <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>385</v>
       </c>
       <c r="F1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" s="1">
         <v>2457426</v>
@@ -1596,10 +1596,10 @@
         <v>1750000</v>
       </c>
       <c r="D2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B3" s="1">
         <v>2381143</v>
@@ -1616,10 +1616,10 @@
         <v>1500000</v>
       </c>
       <c r="D3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E3" t="s">
         <v>235</v>
-      </c>
-      <c r="E3" t="s">
-        <v>236</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="1">
         <v>2191023</v>
@@ -1636,10 +1636,10 @@
         <v>1500000</v>
       </c>
       <c r="D4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" s="1">
         <v>1670875</v>
@@ -1659,7 +1659,7 @@
         <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1679,7 +1679,7 @@
         <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -1699,7 +1699,7 @@
         <v>112</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -1719,7 +1719,7 @@
         <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B9" s="2">
         <v>1308805</v>
@@ -1739,7 +1739,7 @@
         <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -1759,7 +1759,7 @@
         <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B11" s="2">
         <v>1146555</v>
@@ -1779,7 +1779,7 @@
         <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -1799,7 +1799,7 @@
         <v>111</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" s="2">
         <v>900000</v>
@@ -1819,7 +1819,7 @@
         <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B14" s="2">
         <v>900000</v>
@@ -1839,7 +1839,7 @@
         <v>108</v>
       </c>
       <c r="E14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B15" s="2">
         <v>700000</v>
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B16" s="2">
         <v>700000</v>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -1890,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B18" s="2">
         <v>500000</v>
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B20" s="2">
         <v>500000</v>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B21" s="2">
         <v>500000</v>
@@ -1958,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1975,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B24" s="2">
         <v>500000</v>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B25" s="2">
         <v>500000</v>
@@ -2026,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B26" s="2">
         <v>500000</v>
@@ -2043,7 +2043,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B27" s="2">
         <v>500000</v>
@@ -2060,7 +2060,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -2436,7 +2436,7 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2458,10 +2458,10 @@
         <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>385</v>
       </c>
       <c r="F1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2478,7 +2478,7 @@
         <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -2498,7 +2498,7 @@
         <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -2518,7 +2518,7 @@
         <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -2538,7 +2538,7 @@
         <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -2558,7 +2558,7 @@
         <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -2578,7 +2578,7 @@
         <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -2598,7 +2598,7 @@
         <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -2618,7 +2618,7 @@
         <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -2638,7 +2638,7 @@
         <v>108</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -2658,7 +2658,7 @@
         <v>111</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -2675,7 +2675,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -2692,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -2709,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -2743,7 +2743,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -2760,7 +2760,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -2794,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -2811,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
@@ -2828,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -2845,7 +2845,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
@@ -2862,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -2879,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -2896,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -2916,7 +2916,7 @@
         <v>108</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
@@ -2933,7 +2933,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -2950,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -3001,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F32" t="b">
         <v>1</v>
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
@@ -3052,7 +3052,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
@@ -3069,7 +3069,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
@@ -3103,7 +3103,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -3137,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
@@ -3171,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F41" t="b">
         <v>1</v>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F42" t="b">
         <v>1</v>
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -3222,7 +3222,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
@@ -3239,7 +3239,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -3256,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -3273,7 +3273,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
@@ -3290,7 +3290,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
@@ -3324,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
@@ -3341,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -3358,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
@@ -3375,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F54" t="b">
         <v>1</v>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -3426,7 +3426,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
@@ -3443,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -3460,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F58" t="b">
         <v>1</v>
@@ -3477,7 +3477,7 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
@@ -3494,7 +3494,7 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F60" t="b">
         <v>1</v>
@@ -3511,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F61" t="b">
         <v>1</v>
@@ -3528,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F62" t="b">
         <v>1</v>
@@ -3545,7 +3545,7 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F63" t="b">
         <v>1</v>
@@ -3562,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F64" t="b">
         <v>1</v>
@@ -3579,7 +3579,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F65" t="b">
         <v>1</v>
@@ -3596,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F66" t="b">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
@@ -3630,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F68" t="b">
         <v>1</v>
@@ -3647,7 +3647,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F69" t="b">
         <v>1</v>
@@ -3664,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F70" t="b">
         <v>1</v>
@@ -3681,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F71" t="b">
         <v>1</v>
@@ -3698,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F72" t="b">
         <v>1</v>
@@ -3715,7 +3715,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F73" t="b">
         <v>1</v>
@@ -3732,7 +3732,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F74" t="b">
         <v>1</v>
@@ -3749,7 +3749,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F75" t="b">
         <v>1</v>
@@ -3766,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F76" t="b">
         <v>1</v>
@@ -3783,7 +3783,7 @@
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F77" t="b">
         <v>1</v>
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F78" t="b">
         <v>1</v>
@@ -3817,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F79" t="b">
         <v>1</v>
@@ -3834,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F80" t="b">
         <v>1</v>
@@ -3851,7 +3851,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F81" t="b">
         <v>1</v>
@@ -3868,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F82" t="b">
         <v>1</v>
@@ -3885,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F83" t="b">
         <v>1</v>
@@ -3902,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F84" t="b">
         <v>1</v>
@@ -3919,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F85" t="b">
         <v>1</v>
@@ -3936,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F86" t="b">
         <v>1</v>
@@ -3953,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F87" t="b">
         <v>1</v>
@@ -3970,7 +3970,7 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F88" t="b">
         <v>1</v>
@@ -3987,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F89" t="b">
         <v>1</v>
@@ -4004,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F90" t="b">
         <v>1</v>
@@ -4021,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F91" t="b">
         <v>1</v>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F92" t="b">
         <v>1</v>
@@ -4055,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F93" t="b">
         <v>1</v>
@@ -4072,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F94" t="b">
         <v>1</v>
@@ -4089,7 +4089,7 @@
         <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F95" t="b">
         <v>1</v>
@@ -4106,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F96" t="b">
         <v>1</v>
@@ -4123,7 +4123,7 @@
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F97" t="b">
         <v>1</v>
@@ -4140,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F98" t="b">
         <v>1</v>
@@ -4157,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F99" t="b">
         <v>1</v>
@@ -4174,7 +4174,7 @@
         <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F100" t="b">
         <v>1</v>
@@ -4191,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F101" t="b">
         <v>1</v>
@@ -4208,7 +4208,7 @@
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F102" t="b">
         <v>1</v>
@@ -4223,8 +4223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C9B84E-834F-5B4C-8F9E-38BAFB9905EF}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4246,10 +4246,10 @@
         <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>385</v>
       </c>
       <c r="F1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -4263,10 +4263,10 @@
         <v>1750000</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -4274,7 +4274,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3">
         <v>2152057</v>
@@ -4283,10 +4283,10 @@
         <v>1500000</v>
       </c>
       <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
         <v>315</v>
-      </c>
-      <c r="E3" t="s">
-        <v>316</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -4306,7 +4306,7 @@
         <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -4323,10 +4323,10 @@
         <v>1000000</v>
       </c>
       <c r="D5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -4346,7 +4346,7 @@
         <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -4363,10 +4363,10 @@
         <v>500000</v>
       </c>
       <c r="D7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -4374,7 +4374,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8">
         <v>1191534</v>
@@ -4383,10 +4383,10 @@
         <v>500000</v>
       </c>
       <c r="D8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B9">
         <v>1098628</v>
@@ -4403,10 +4403,10 @@
         <v>750000</v>
       </c>
       <c r="D9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -4414,7 +4414,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B10">
         <v>978671</v>
@@ -4426,7 +4426,7 @@
         <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -4434,7 +4434,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B11">
         <v>901335</v>
@@ -4443,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -4460,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -4468,7 +4468,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B13">
         <v>825276</v>
@@ -4477,10 +4477,10 @@
         <v>500000</v>
       </c>
       <c r="D13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -4488,7 +4488,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B14">
         <v>801564</v>
@@ -4497,7 +4497,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -4514,7 +4514,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -4548,7 +4548,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B18">
         <v>557688</v>
@@ -4565,7 +4565,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -4582,7 +4582,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
@@ -4607,7 +4607,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B21">
         <v>534267</v>
@@ -4616,7 +4616,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B22">
         <v>529910</v>
@@ -4633,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
@@ -4650,7 +4650,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -4667,7 +4667,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -4701,7 +4701,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B27">
         <v>484750</v>
@@ -4718,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -4726,7 +4726,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B28">
         <v>483928</v>
@@ -4735,7 +4735,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -4743,7 +4743,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B29">
         <v>473026</v>
@@ -4752,7 +4752,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -4769,7 +4769,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B31">
         <v>459896</v>
@@ -4786,7 +4786,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
@@ -4803,7 +4803,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F32" t="b">
         <v>1</v>
@@ -4811,7 +4811,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B33">
         <v>442551</v>
@@ -4820,7 +4820,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B34">
         <v>427663</v>
@@ -4837,7 +4837,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B35">
         <v>424722</v>
@@ -4854,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
@@ -4871,7 +4871,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B37">
         <v>417995</v>
@@ -4888,7 +4888,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B38">
         <v>416842</v>
@@ -4905,7 +4905,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -4913,7 +4913,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B39">
         <v>414638</v>
@@ -4922,7 +4922,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -4939,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
@@ -4947,7 +4947,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B41">
         <v>409573</v>
@@ -4956,7 +4956,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F41" t="b">
         <v>1</v>
@@ -4964,7 +4964,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B42">
         <v>382315</v>
@@ -4973,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F42" t="b">
         <v>1</v>
@@ -4990,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B44">
         <v>377494</v>
@@ -5007,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
@@ -5015,7 +5015,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B45">
         <v>370770</v>
@@ -5024,7 +5024,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -5032,7 +5032,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B46">
         <v>368844</v>
@@ -5041,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B47">
         <v>368745</v>
@@ -5058,7 +5058,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
@@ -5066,7 +5066,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B48">
         <v>368014</v>
@@ -5075,7 +5075,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
@@ -5083,7 +5083,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B49">
         <v>365752</v>
@@ -5092,7 +5092,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
@@ -5100,7 +5100,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B50">
         <v>362483</v>
@@ -5109,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
@@ -5126,7 +5126,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -5134,7 +5134,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B52">
         <v>352852</v>
@@ -5143,7 +5143,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B53">
         <v>350022</v>
@@ -5160,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
@@ -5168,7 +5168,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B54">
         <v>342128</v>
@@ -5177,7 +5177,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F54" t="b">
         <v>1</v>
@@ -5194,7 +5194,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -5202,7 +5202,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B56">
         <v>339964</v>
@@ -5211,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
@@ -5219,7 +5219,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B57">
         <v>333239</v>
@@ -5228,7 +5228,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -5236,7 +5236,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B58">
         <v>333175</v>
@@ -5245,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F58" t="b">
         <v>1</v>
@@ -5262,7 +5262,7 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F60" t="b">
         <v>1</v>
@@ -5287,7 +5287,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B61">
         <v>325723</v>
@@ -5296,7 +5296,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F61" t="b">
         <v>1</v>
@@ -5313,7 +5313,7 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F62" t="b">
         <v>1</v>
@@ -5330,7 +5330,7 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F63" t="b">
         <v>1</v>
@@ -5338,7 +5338,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B64">
         <v>321013</v>
@@ -5347,7 +5347,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F64" t="b">
         <v>1</v>
@@ -5355,7 +5355,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B65">
         <v>314708</v>
@@ -5364,7 +5364,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F65" t="b">
         <v>1</v>
@@ -5381,7 +5381,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F66" t="b">
         <v>1</v>
@@ -5389,7 +5389,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B67">
         <v>313489</v>
@@ -5398,7 +5398,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
@@ -5415,7 +5415,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F68" t="b">
         <v>1</v>
@@ -5423,7 +5423,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B69">
         <v>312411</v>
@@ -5432,7 +5432,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F69" t="b">
         <v>1</v>
@@ -5449,7 +5449,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F70" t="b">
         <v>1</v>
@@ -5457,7 +5457,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B71">
         <v>300017</v>
@@ -5466,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F71" t="b">
         <v>1</v>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B72">
         <v>291335</v>
@@ -5483,7 +5483,7 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F72" t="b">
         <v>1</v>
@@ -5491,7 +5491,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B73">
         <v>288414</v>
@@ -5500,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F73" t="b">
         <v>1</v>
@@ -5517,7 +5517,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F74" t="b">
         <v>1</v>
@@ -5534,7 +5534,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F75" t="b">
         <v>1</v>
@@ -5542,7 +5542,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B76">
         <v>276802</v>
@@ -5551,7 +5551,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F76" t="b">
         <v>1</v>
@@ -5559,7 +5559,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B77">
         <v>274561</v>
@@ -5568,7 +5568,7 @@
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F77" t="b">
         <v>1</v>
@@ -5576,7 +5576,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B78">
         <v>271783</v>
@@ -5585,7 +5585,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F78" t="b">
         <v>1</v>
@@ -5602,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F79" t="b">
         <v>1</v>
@@ -5610,7 +5610,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B80">
         <v>263114</v>
@@ -5619,7 +5619,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F80" t="b">
         <v>1</v>
@@ -5627,7 +5627,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B81">
         <v>261138</v>
@@ -5636,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F81" t="b">
         <v>1</v>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B82">
         <v>260489</v>
@@ -5653,7 +5653,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F82" t="b">
         <v>1</v>
@@ -5661,7 +5661,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B83">
         <v>256296</v>
@@ -5670,7 +5670,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F83" t="b">
         <v>1</v>
@@ -5678,7 +5678,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B84">
         <v>255500</v>
@@ -5687,7 +5687,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F84" t="b">
         <v>1</v>
@@ -5695,7 +5695,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B85">
         <v>254824</v>
@@ -5704,7 +5704,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F85" t="b">
         <v>1</v>
@@ -5721,7 +5721,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F86" t="b">
         <v>1</v>
@@ -5729,7 +5729,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B87">
         <v>246858</v>
@@ -5738,7 +5738,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F87" t="b">
         <v>1</v>
@@ -5746,7 +5746,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B88">
         <v>246313</v>
@@ -5755,7 +5755,7 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F88" t="b">
         <v>1</v>
@@ -5763,7 +5763,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B89">
         <v>245805</v>
@@ -5772,7 +5772,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F89" t="b">
         <v>1</v>
@@ -5789,7 +5789,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F90" t="b">
         <v>1</v>
@@ -5797,7 +5797,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B91">
         <v>243471</v>
@@ -5806,7 +5806,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F91" t="b">
         <v>1</v>
@@ -5823,7 +5823,7 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F92" t="b">
         <v>1</v>
@@ -5831,7 +5831,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B93">
         <v>242569</v>
@@ -5840,7 +5840,7 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F93" t="b">
         <v>1</v>
@@ -5848,7 +5848,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B94">
         <v>241935</v>
@@ -5857,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F94" t="b">
         <v>1</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B95">
         <v>241789</v>
@@ -5874,7 +5874,7 @@
         <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F95" t="b">
         <v>1</v>
@@ -5891,7 +5891,7 @@
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F96" t="b">
         <v>1</v>
@@ -5899,7 +5899,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B97">
         <v>240856</v>
@@ -5908,7 +5908,7 @@
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F97" t="b">
         <v>1</v>
@@ -5916,7 +5916,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B98">
         <v>239663</v>
@@ -5925,7 +5925,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F98" t="b">
         <v>1</v>
@@ -5942,7 +5942,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F99" t="b">
         <v>1</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B100">
         <v>236029</v>
@@ -5959,7 +5959,7 @@
         <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F100" t="b">
         <v>1</v>
@@ -5967,7 +5967,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B101">
         <v>232819</v>
@@ -5976,7 +5976,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F101" t="b">
         <v>1</v>
@@ -5984,7 +5984,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B102">
         <v>232549</v>
@@ -5993,7 +5993,7 @@
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F102" t="b">
         <v>1</v>

</xml_diff>